<commit_message>
Created logic for harvester.
</commit_message>
<xml_diff>
--- a/Content/Harvester/Harvester_Infos.xlsx
+++ b/Content/Harvester/Harvester_Infos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Kartar</t>
   </si>
@@ -22,67 +22,28 @@
     <t>4000</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>t</t>
+    <t>101 HP</t>
+  </si>
+  <si>
+    <t>14 Feet</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>Self Propelled</t>
+  </si>
+  <si>
+    <t>Multicrop</t>
+  </si>
+  <si>
+    <t>Kartar 4000 Tractor Harvester is an efficient machine for farming in India. The farmers are extensively using Kartar 4000 Multicrop harvester for their farms. In addition, Kartar 4000 harvester features are also excellent. That’s why the Kartar 4000 harvester machine is one of India's most preferred farming machines. Kartar 4000 price 2024 is also valuable for farmers. Moreover, the Kartar 4000 harvester machine is filled with highly modern technology to serve better in the field.
+Kartar 4000 Multicrop Combine Harvester Price
+Kartar 4000 Multicrop combine harvester price is valuable to the Indian farmers. You can also get a complete Kartar 4000 combine harvester price list at Tractor Junction. On the other hand, the Kartar 4000 combine on road price can differ from state to state due to several factors.
+Kartar 4000 Harvester Features
+Let’s know the Kartar 4000 harvester features. The working efficiency and performance of Kartar 4000 Tractor Harvester are also excellent. The engine of this Kartar 4000 has enormous power and comes at value for money Kartar 4000 combine price. So, let’s know more about Kartar 4000 Multicrop harvester at Tractor Junction.
+Kartar 4000 Combine Harvester Price at Tractor Junction
+You can get a reliable Kartar 4000 combine price at Tractor Junction. Here we are with complete details of this harvester, including Kartar 4000 combine price 2024, specifications and others. Apart from this, you can also call us to get genuine Kartar 4000 combine on road price at your place.</t>
   </si>
   <si>
     <t>Brand</t>
@@ -91,22 +52,25 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Model Name</t>
-  </si>
-  <si>
     <t>Power</t>
   </si>
   <si>
-    <t>Cutter Bar – Width</t>
-  </si>
-  <si>
-    <t>No Of Cylinder</t>
-  </si>
-  <si>
-    <t>Power Source</t>
+    <t>Cutter_Width</t>
+  </si>
+  <si>
+    <t>No_of_Cylinder</t>
+  </si>
+  <si>
+    <t>Power_Sorce</t>
   </si>
   <si>
     <t>Crop</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Engine_Rated_RPM</t>
   </si>
 </sst>
 </file>
@@ -462,39 +426,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -505,150 +472,19 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="D7" t="s">
         <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="G15" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>